<commit_message>
Update core game filter questions, survey plan, and analysis fw; Add survey link to README
</commit_message>
<xml_diff>
--- a/method/CoreGame - titles and filter questions.xlsx
+++ b/method/CoreGame - titles and filter questions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\GitHub\MACS30200proj\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\GitHub\MAPSS-Thesis\method\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14646" yWindow="0" windowWidth="30702" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="19170" yWindow="0" windowWidth="30700" windowHeight="16980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="213">
   <si>
     <t>Game</t>
   </si>
@@ -778,7 +778,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -833,21 +833,61 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Yu Gothic UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6E7E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -872,7 +912,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -890,6 +930,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -914,6 +964,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF6E7E6"/>
+      <color rgb="FFFBF3F3"/>
+      <color rgb="FFF5E4E3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1249,25 +1306,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.09765625" customWidth="1"/>
-    <col min="2" max="2" width="26.84765625" customWidth="1"/>
-    <col min="3" max="3" width="19.6484375" customWidth="1"/>
-    <col min="4" max="4" width="75.6484375" customWidth="1"/>
-    <col min="5" max="5" width="81.1484375" customWidth="1"/>
-    <col min="6" max="6" width="25.546875" customWidth="1"/>
+    <col min="1" max="1" width="5.08203125" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="75.6640625" customWidth="1"/>
+    <col min="5" max="5" width="81.1640625" customWidth="1"/>
+    <col min="6" max="6" width="25.58203125" customWidth="1"/>
     <col min="8" max="8" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>91</v>
       </c>
@@ -1293,7 +1350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1320,7 +1377,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1347,7 +1404,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1374,7 +1431,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1401,7 +1458,7 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1428,7 +1485,7 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1455,7 +1512,7 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1482,7 +1539,7 @@
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1509,7 +1566,7 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1536,7 +1593,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1563,7 +1620,7 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1590,7 +1647,7 @@
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1617,7 +1674,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1644,7 +1701,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1671,7 +1728,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1697,7 +1754,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1723,7 +1780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1749,7 +1806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1775,7 +1832,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1801,7 +1858,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1827,7 +1884,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1853,7 +1910,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1879,7 +1936,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1905,7 +1962,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1931,7 +1988,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1957,8 +2014,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.6"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1981,7 +2038,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2004,7 +2061,7 @@
         <v>14.98</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2027,7 +2084,7 @@
         <v>6.48</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2050,7 +2107,7 @@
         <v>8.4600000000000009</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2073,7 +2130,7 @@
         <v>8.86</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2096,7 +2153,7 @@
         <v>20.16</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2119,7 +2176,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2142,7 +2199,7 @@
         <v>10.119999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2165,7 +2222,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2188,7 +2245,7 @@
         <v>5.21</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2211,7 +2268,7 @@
         <v>9.6199999999999992</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2234,7 +2291,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2257,7 +2314,7 @@
         <v>5.82</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2280,7 +2337,7 @@
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2303,11 +2360,11 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D44" s="4"/>
     </row>
   </sheetData>
@@ -2323,138 +2380,223 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:C25"/>
+  <dimension ref="B1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="6" width="34.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="2:7" ht="16" x14ac:dyDescent="0.35">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="9"/>
+      <c r="C3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="9"/>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B5" s="9"/>
+      <c r="C5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B6" s="9"/>
+      <c r="C6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C2" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C3" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C4" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C5" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C6" s="5" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B7" s="9"/>
+      <c r="C7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B8" s="9"/>
+      <c r="C8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B9" s="9"/>
+      <c r="C9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="2:7" ht="16" x14ac:dyDescent="0.35">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B11" s="9"/>
+      <c r="C11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C7" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C8" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C10" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C12" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C18" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C19" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C20" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C21" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C22" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C24" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.6">
-      <c r="C25" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E11" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="2:7" ht="16" x14ac:dyDescent="0.35">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B13" s="9"/>
+      <c r="C13" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="2:7" ht="16" x14ac:dyDescent="0.35">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="9"/>
+      <c r="C15" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update core games to 50
</commit_message>
<xml_diff>
--- a/method/CoreGame - titles and filter questions.xlsx
+++ b/method/CoreGame - titles and filter questions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\GitHub\MAPSS-Thesis\method\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\GitHub\MACS30200proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19170" yWindow="0" windowWidth="30700" windowHeight="16980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="30470" yWindow="0" windowWidth="30700" windowHeight="16980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="262">
   <si>
     <t>Game</t>
   </si>
@@ -480,12 +480,6 @@
     </r>
   </si>
   <si>
-    <t>The main antagonist in the game Half-life 2 is/are:</t>
-  </si>
-  <si>
-    <t>What are the antagonists in Resident Evil 5?</t>
-  </si>
-  <si>
     <t>In League of Legends, how many Control Wards can a TEAM have on the map at once?</t>
   </si>
   <si>
@@ -513,9 +507,6 @@
     <t>Superstar Mode, Player Story Mode, Single Player Mode, Career Mode</t>
   </si>
   <si>
-    <t>Star Wars: Battlefront is based mainly on which episode in the Star Wars franchise?</t>
-  </si>
-  <si>
     <t>StarCraft II: Wings of Liberty features the story of which of the following races?</t>
   </si>
   <si>
@@ -613,9 +604,6 @@
   </si>
   <si>
     <t>In WOW, which of the followings is a Class?</t>
-  </si>
-  <si>
-    <t>In Pokemon Red and Blue, a primary antagonist is/are:</t>
   </si>
   <si>
     <t>In The Legend of Zelda: Ocarina of Time, the name of the protagonist is:</t>
@@ -657,30 +645,9 @@
     </r>
   </si>
   <si>
-    <t>In New Super Mario Bros, the protagonist collects:</t>
-  </si>
-  <si>
     <t>In Donkey Kong Country Returns, who is not a Kong character?</t>
   </si>
   <si>
-    <t>Regarding The Elder Scrolls V: Skyrim, Skyrim refers to:</t>
-  </si>
-  <si>
-    <r>
-      <t>In Brain Age: Train Your Brain in Minutes, which of the following is not a primary test focus?</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
     <t>spatial skill, calculation skill, reading skill, memory skill</t>
   </si>
   <si>
@@ -688,9 +655,6 @@
   </si>
   <si>
     <t>In Kingdom Hearts, which character does not directly engage in battles?</t>
-  </si>
-  <si>
-    <t>In Dragon Quest VIII: Journey of the Cursed King, which of the following is a major weapon used by one of the protagonists?</t>
   </si>
   <si>
     <r>
@@ -708,21 +672,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>In the original LittleBigPlanet game, players are unable to perform which of the following?</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
     <t>In God of War III, which of the following is untrue about Krato's weapon?</t>
   </si>
   <si>
@@ -765,20 +714,206 @@
     <t>It is nicknamed GT3 by players, Player passes a license test to start the game, Player manages a racing car team in the game, It mainly features Formula One cars</t>
   </si>
   <si>
-    <t>a world, a big island, a magical scroll, one of the protagonists</t>
-  </si>
-  <si>
     <t>music record sales, bands, boss battles, songs</t>
   </si>
   <si>
     <t>It is a pair of long swords, It is replaced several times across the game, It is attached by a chain, It gives Krato magiical abilities</t>
+  </si>
+  <si>
+    <t>In The Elder Scrolls V: Skyrim, Skyrim refers to:</t>
+  </si>
+  <si>
+    <t>In Pokemon Red and Blue, a primary enemy to the main characters is/are:</t>
+  </si>
+  <si>
+    <t>In New Super Mario Bros, the player character collects:</t>
+  </si>
+  <si>
+    <t>The enemy to the main character in the game Half-life 2 is/are:</t>
+  </si>
+  <si>
+    <t>What are the enemies to the main characters in Resident Evil 5?</t>
+  </si>
+  <si>
+    <t>In Brain Age: Train Your Brain in Minutes, which of the following is not primarily tested?</t>
+  </si>
+  <si>
+    <t> Star Wars: Battlefront is mainly based on which episode in the Star Wars series?</t>
+  </si>
+  <si>
+    <t>In Dragon Quest VIII: Journey of the Cursed King, which of the following is a primary weapon used by one of the main characters?</t>
+  </si>
+  <si>
+    <r>
+      <t>In LittleBigPlanet, players are unable to perform which of the following?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>an entire world, a sorcery, a magical scroll, the main character</t>
+  </si>
+  <si>
+    <t>Shooter/RPG</t>
+  </si>
+  <si>
+    <t>Splatoon</t>
+  </si>
+  <si>
+    <t>Shooter/online</t>
+  </si>
+  <si>
+    <t>Wii Fit</t>
+  </si>
+  <si>
+    <t>Exercise</t>
+  </si>
+  <si>
+    <t>Warcraft II: Tides of Darkness</t>
+  </si>
+  <si>
+    <t>Strategy/online</t>
+  </si>
+  <si>
+    <t>The Last of Us</t>
+  </si>
+  <si>
+    <t>ARPG/rogue</t>
+  </si>
+  <si>
+    <t>Professor Layton and the Curious Village</t>
+  </si>
+  <si>
+    <t>Puzzle/Adventure</t>
+  </si>
+  <si>
+    <t>Pokémon GO</t>
+  </si>
+  <si>
+    <t>Candy Crush Saga</t>
+  </si>
+  <si>
+    <t>Clash of Clans</t>
+  </si>
+  <si>
+    <t>Hearthstone</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Strategy/Simulation/online</t>
+  </si>
+  <si>
+    <t>Collection/RPG</t>
+  </si>
+  <si>
+    <t>fungi, a nuclear war, radiation, a super bacteria</t>
+  </si>
+  <si>
+    <t>fungi</t>
+  </si>
+  <si>
+    <t>In Splatoon, what is incorrect about shapeshifting?</t>
+  </si>
+  <si>
+    <t>You shoot ink to change environment's color, You become a squid, You swim within the ink, You can replenish your ink supply</t>
+  </si>
+  <si>
+    <t>You shoot ink to change environment's color</t>
+  </si>
+  <si>
+    <t>What is correct about the special gadget used with Wii Fit:</t>
+  </si>
+  <si>
+    <t>It detects body's center of balance</t>
+  </si>
+  <si>
+    <t>crystal</t>
+  </si>
+  <si>
+    <t>What is not an essential resource in Warcraft II: Tides of Darkness?</t>
+  </si>
+  <si>
+    <t>Monster Hunter Freedom Unite</t>
+  </si>
+  <si>
+    <t>It is a place players hatch Pokémon eggs, It is a place players battle rival Pokémon, It is a place players train his/her own Pokémon, It can be leveled up</t>
+  </si>
+  <si>
+    <t>It is a place players hatch Pokémon eggs</t>
+  </si>
+  <si>
+    <t>In Candy Crush Saga, what is true about a chocolate bomb?</t>
+  </si>
+  <si>
+    <t>It can be matched with other special candies to create combo effects; It is created by matching four pieces of candy of the same color; It can be triggered by player tapping on it; It removes all candies on the current screen</t>
+  </si>
+  <si>
+    <t>It can be matched with other special candies to create combo effects</t>
+  </si>
+  <si>
+    <t>Dragon Knight; Balloon; P.E.K.K.A; Hog Rider</t>
+  </si>
+  <si>
+    <t>Archer</t>
+  </si>
+  <si>
+    <t>Archer; Paladin; Warlock; Rogue</t>
+  </si>
+  <si>
+    <t>Dragon Knight</t>
+  </si>
+  <si>
+    <t>Which of the folloing is not a hero Class in Hearthstone?</t>
+  </si>
+  <si>
+    <t>What description is incorrect about Luke Triton in Professor Layton and the Curious Village?</t>
+  </si>
+  <si>
+    <t>He is Layton's second son; He aspires to be a gentleman like Layton; He can talk to animals; He has very good appetite</t>
+  </si>
+  <si>
+    <t>In Monster Hunter Freedom Unite, what animal can you hire to fight with you?</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>cat, eagle, bear, hound</t>
+  </si>
+  <si>
+    <t>In The Last of Us, what is the source of world's devastation?</t>
+  </si>
+  <si>
+    <t>It detects body's center of balance, It evaluates both hands' movement, It measures body temperature, It estimates heart rate</t>
+  </si>
+  <si>
+    <t>crystal, wood, gold, worker</t>
+  </si>
+  <si>
+    <t>He is Layton's second son; He aspires to be a gentleman like Layton; He can talk to animals; He has a big appetite</t>
+  </si>
+  <si>
+    <t>In Pokémon GO, what is incorrect about Gym?</t>
+  </si>
+  <si>
+    <t>What is not a troop unit you can train in Clash of Clans?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -833,61 +968,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Yu Gothic UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6E7E6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -912,7 +1007,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -930,16 +1025,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -964,13 +1049,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFF6E7E6"/>
-      <color rgb="FFFBF3F3"/>
-      <color rgb="FFF5E4E3"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1304,13 +1382,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1361,10 +1439,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>95</v>
@@ -1391,7 +1469,7 @@
         <v>94</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>98</v>
@@ -1415,10 +1493,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>99</v>
@@ -1442,10 +1520,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>118</v>
@@ -1469,10 +1547,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>100</v>
@@ -1496,10 +1574,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>96</v>
@@ -1523,10 +1601,10 @@
         <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>101</v>
@@ -1550,10 +1628,10 @@
         <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>102</v>
@@ -1580,7 +1658,7 @@
         <v>127</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>103</v>
@@ -1604,10 +1682,10 @@
         <v>22</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>97</v>
@@ -1631,10 +1709,10 @@
         <v>32</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>104</v>
@@ -1658,10 +1736,10 @@
         <v>35</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>105</v>
@@ -1688,7 +1766,7 @@
         <v>128</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>106</v>
@@ -1715,7 +1793,7 @@
         <v>129</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>107</v>
@@ -1742,7 +1820,7 @@
         <v>130</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>108</v>
@@ -1768,7 +1846,7 @@
         <v>131</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>109</v>
@@ -1791,10 +1869,10 @@
         <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>110</v>
@@ -1817,10 +1895,10 @@
         <v>49</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>111</v>
@@ -1846,7 +1924,7 @@
         <v>132</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>112</v>
@@ -1869,10 +1947,10 @@
         <v>78</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>113</v>
@@ -1898,7 +1976,7 @@
         <v>133</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>115</v>
@@ -1921,10 +1999,10 @@
         <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>114</v>
@@ -1950,7 +2028,7 @@
         <v>134</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>117</v>
@@ -1973,10 +2051,10 @@
         <v>22</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>135</v>
+        <v>206</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>119</v>
@@ -1999,10 +2077,10 @@
         <v>64</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>136</v>
+        <v>207</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>116</v>
@@ -2026,10 +2104,10 @@
         <v>89</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F28" s="4">
         <v>5</v>
@@ -2049,13 +2127,13 @@
         <v>35</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G29" s="4">
         <v>14.98</v>
@@ -2072,10 +2150,10 @@
         <v>78</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>120</v>
@@ -2095,10 +2173,10 @@
         <v>22</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>121</v>
@@ -2118,13 +2196,13 @@
         <v>85</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G32" s="4">
         <v>8.86</v>
@@ -2141,13 +2219,13 @@
         <v>47</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G33" s="4">
         <v>20.16</v>
@@ -2164,10 +2242,10 @@
         <v>6</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>122</v>
@@ -2187,10 +2265,10 @@
         <v>79</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>123</v>
@@ -2210,10 +2288,10 @@
         <v>80</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>124</v>
@@ -2233,13 +2311,13 @@
         <v>12</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G37" s="4">
         <v>5.21</v>
@@ -2256,10 +2334,10 @@
         <v>28</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>125</v>
@@ -2279,13 +2357,13 @@
         <v>81</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G39" s="4">
         <v>4.53</v>
@@ -2302,10 +2380,10 @@
         <v>82</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>126</v>
@@ -2325,13 +2403,13 @@
         <v>83</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G41" s="4">
         <v>4.8099999999999996</v>
@@ -2348,13 +2426,13 @@
         <v>84</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G42" s="4">
         <v>4.91</v>
@@ -2365,7 +2443,237 @@
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D44" s="4"/>
+      <c r="A44" s="1">
+        <v>41</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="G44" s="4">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>42</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="G45" s="4">
+        <v>4.6500000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>43</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G46" s="4">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>44</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G47" s="4">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>45</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G48" s="4">
+        <v>5.48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>46</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G49" s="4">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>47</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="F50" t="s">
+        <v>242</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>48</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>49</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>50</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F53" t="s">
+        <v>247</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C54" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2380,223 +2688,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G27"/>
+  <dimension ref="C1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="6" width="34.25" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="2:7" ht="16" x14ac:dyDescent="0.35">
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+    <row r="1" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="9"/>
-      <c r="C3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B4" s="9"/>
-      <c r="C4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B5" s="9"/>
-      <c r="C5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B6" s="9"/>
-      <c r="C6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B7" s="9"/>
-      <c r="C7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B8" s="9"/>
-      <c r="C8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B9" s="9"/>
-      <c r="C9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="16" x14ac:dyDescent="0.35">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B11" s="9"/>
-      <c r="C11" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="2:7" ht="16" x14ac:dyDescent="0.35">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B13" s="9"/>
-      <c r="C13" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="2:7" ht="16" x14ac:dyDescent="0.35">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B15" s="9"/>
-      <c r="C15" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C27" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update core games to 50; upload survey plan and instruction; upload lit review fw
</commit_message>
<xml_diff>
--- a/method/CoreGame - titles and filter questions.xlsx
+++ b/method/CoreGame - titles and filter questions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\GitHub\MAPSS-Thesis\method\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\GitHub\MACS30200proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19170" yWindow="0" windowWidth="30700" windowHeight="16980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="30470" yWindow="0" windowWidth="30700" windowHeight="16980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="262">
   <si>
     <t>Game</t>
   </si>
@@ -480,12 +480,6 @@
     </r>
   </si>
   <si>
-    <t>The main antagonist in the game Half-life 2 is/are:</t>
-  </si>
-  <si>
-    <t>What are the antagonists in Resident Evil 5?</t>
-  </si>
-  <si>
     <t>In League of Legends, how many Control Wards can a TEAM have on the map at once?</t>
   </si>
   <si>
@@ -513,9 +507,6 @@
     <t>Superstar Mode, Player Story Mode, Single Player Mode, Career Mode</t>
   </si>
   <si>
-    <t>Star Wars: Battlefront is based mainly on which episode in the Star Wars franchise?</t>
-  </si>
-  <si>
     <t>StarCraft II: Wings of Liberty features the story of which of the following races?</t>
   </si>
   <si>
@@ -613,9 +604,6 @@
   </si>
   <si>
     <t>In WOW, which of the followings is a Class?</t>
-  </si>
-  <si>
-    <t>In Pokemon Red and Blue, a primary antagonist is/are:</t>
   </si>
   <si>
     <t>In The Legend of Zelda: Ocarina of Time, the name of the protagonist is:</t>
@@ -657,30 +645,9 @@
     </r>
   </si>
   <si>
-    <t>In New Super Mario Bros, the protagonist collects:</t>
-  </si>
-  <si>
     <t>In Donkey Kong Country Returns, who is not a Kong character?</t>
   </si>
   <si>
-    <t>Regarding The Elder Scrolls V: Skyrim, Skyrim refers to:</t>
-  </si>
-  <si>
-    <r>
-      <t>In Brain Age: Train Your Brain in Minutes, which of the following is not a primary test focus?</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
     <t>spatial skill, calculation skill, reading skill, memory skill</t>
   </si>
   <si>
@@ -688,9 +655,6 @@
   </si>
   <si>
     <t>In Kingdom Hearts, which character does not directly engage in battles?</t>
-  </si>
-  <si>
-    <t>In Dragon Quest VIII: Journey of the Cursed King, which of the following is a major weapon used by one of the protagonists?</t>
   </si>
   <si>
     <r>
@@ -708,21 +672,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>In the original LittleBigPlanet game, players are unable to perform which of the following?</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
     <t>In God of War III, which of the following is untrue about Krato's weapon?</t>
   </si>
   <si>
@@ -765,20 +714,206 @@
     <t>It is nicknamed GT3 by players, Player passes a license test to start the game, Player manages a racing car team in the game, It mainly features Formula One cars</t>
   </si>
   <si>
-    <t>a world, a big island, a magical scroll, one of the protagonists</t>
-  </si>
-  <si>
     <t>music record sales, bands, boss battles, songs</t>
   </si>
   <si>
     <t>It is a pair of long swords, It is replaced several times across the game, It is attached by a chain, It gives Krato magiical abilities</t>
+  </si>
+  <si>
+    <t>In The Elder Scrolls V: Skyrim, Skyrim refers to:</t>
+  </si>
+  <si>
+    <t>In Pokemon Red and Blue, a primary enemy to the main characters is/are:</t>
+  </si>
+  <si>
+    <t>In New Super Mario Bros, the player character collects:</t>
+  </si>
+  <si>
+    <t>The enemy to the main character in the game Half-life 2 is/are:</t>
+  </si>
+  <si>
+    <t>What are the enemies to the main characters in Resident Evil 5?</t>
+  </si>
+  <si>
+    <t>In Brain Age: Train Your Brain in Minutes, which of the following is not primarily tested?</t>
+  </si>
+  <si>
+    <t> Star Wars: Battlefront is mainly based on which episode in the Star Wars series?</t>
+  </si>
+  <si>
+    <t>In Dragon Quest VIII: Journey of the Cursed King, which of the following is a primary weapon used by one of the main characters?</t>
+  </si>
+  <si>
+    <r>
+      <t>In LittleBigPlanet, players are unable to perform which of the following?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>an entire world, a sorcery, a magical scroll, the main character</t>
+  </si>
+  <si>
+    <t>Shooter/RPG</t>
+  </si>
+  <si>
+    <t>Splatoon</t>
+  </si>
+  <si>
+    <t>Shooter/online</t>
+  </si>
+  <si>
+    <t>Wii Fit</t>
+  </si>
+  <si>
+    <t>Exercise</t>
+  </si>
+  <si>
+    <t>Warcraft II: Tides of Darkness</t>
+  </si>
+  <si>
+    <t>Strategy/online</t>
+  </si>
+  <si>
+    <t>The Last of Us</t>
+  </si>
+  <si>
+    <t>ARPG/rogue</t>
+  </si>
+  <si>
+    <t>Professor Layton and the Curious Village</t>
+  </si>
+  <si>
+    <t>Puzzle/Adventure</t>
+  </si>
+  <si>
+    <t>Pokémon GO</t>
+  </si>
+  <si>
+    <t>Candy Crush Saga</t>
+  </si>
+  <si>
+    <t>Clash of Clans</t>
+  </si>
+  <si>
+    <t>Hearthstone</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Strategy/Simulation/online</t>
+  </si>
+  <si>
+    <t>Collection/RPG</t>
+  </si>
+  <si>
+    <t>fungi, a nuclear war, radiation, a super bacteria</t>
+  </si>
+  <si>
+    <t>fungi</t>
+  </si>
+  <si>
+    <t>In Splatoon, what is incorrect about shapeshifting?</t>
+  </si>
+  <si>
+    <t>You shoot ink to change environment's color, You become a squid, You swim within the ink, You can replenish your ink supply</t>
+  </si>
+  <si>
+    <t>You shoot ink to change environment's color</t>
+  </si>
+  <si>
+    <t>What is correct about the special gadget used with Wii Fit:</t>
+  </si>
+  <si>
+    <t>It detects body's center of balance</t>
+  </si>
+  <si>
+    <t>crystal</t>
+  </si>
+  <si>
+    <t>What is not an essential resource in Warcraft II: Tides of Darkness?</t>
+  </si>
+  <si>
+    <t>Monster Hunter Freedom Unite</t>
+  </si>
+  <si>
+    <t>It is a place players hatch Pokémon eggs, It is a place players battle rival Pokémon, It is a place players train his/her own Pokémon, It can be leveled up</t>
+  </si>
+  <si>
+    <t>It is a place players hatch Pokémon eggs</t>
+  </si>
+  <si>
+    <t>In Candy Crush Saga, what is true about a chocolate bomb?</t>
+  </si>
+  <si>
+    <t>It can be matched with other special candies to create combo effects; It is created by matching four pieces of candy of the same color; It can be triggered by player tapping on it; It removes all candies on the current screen</t>
+  </si>
+  <si>
+    <t>It can be matched with other special candies to create combo effects</t>
+  </si>
+  <si>
+    <t>Dragon Knight; Balloon; P.E.K.K.A; Hog Rider</t>
+  </si>
+  <si>
+    <t>Archer</t>
+  </si>
+  <si>
+    <t>Archer; Paladin; Warlock; Rogue</t>
+  </si>
+  <si>
+    <t>Dragon Knight</t>
+  </si>
+  <si>
+    <t>Which of the folloing is not a hero Class in Hearthstone?</t>
+  </si>
+  <si>
+    <t>What description is incorrect about Luke Triton in Professor Layton and the Curious Village?</t>
+  </si>
+  <si>
+    <t>He is Layton's second son; He aspires to be a gentleman like Layton; He can talk to animals; He has very good appetite</t>
+  </si>
+  <si>
+    <t>In Monster Hunter Freedom Unite, what animal can you hire to fight with you?</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>cat, eagle, bear, hound</t>
+  </si>
+  <si>
+    <t>In The Last of Us, what is the source of world's devastation?</t>
+  </si>
+  <si>
+    <t>It detects body's center of balance, It evaluates both hands' movement, It measures body temperature, It estimates heart rate</t>
+  </si>
+  <si>
+    <t>crystal, wood, gold, worker</t>
+  </si>
+  <si>
+    <t>He is Layton's second son; He aspires to be a gentleman like Layton; He can talk to animals; He has a big appetite</t>
+  </si>
+  <si>
+    <t>In Pokémon GO, what is incorrect about Gym?</t>
+  </si>
+  <si>
+    <t>What is not a troop unit you can train in Clash of Clans?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -833,61 +968,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Yu Gothic UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6E7E6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -912,7 +1007,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -930,16 +1025,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -964,13 +1049,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFF6E7E6"/>
-      <color rgb="FFFBF3F3"/>
-      <color rgb="FFF5E4E3"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1304,13 +1382,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1361,10 +1439,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>95</v>
@@ -1391,7 +1469,7 @@
         <v>94</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>98</v>
@@ -1415,10 +1493,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>99</v>
@@ -1442,10 +1520,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>118</v>
@@ -1469,10 +1547,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>100</v>
@@ -1496,10 +1574,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>96</v>
@@ -1523,10 +1601,10 @@
         <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>101</v>
@@ -1550,10 +1628,10 @@
         <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>102</v>
@@ -1580,7 +1658,7 @@
         <v>127</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>103</v>
@@ -1604,10 +1682,10 @@
         <v>22</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>97</v>
@@ -1631,10 +1709,10 @@
         <v>32</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>104</v>
@@ -1658,10 +1736,10 @@
         <v>35</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>105</v>
@@ -1688,7 +1766,7 @@
         <v>128</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>106</v>
@@ -1715,7 +1793,7 @@
         <v>129</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>107</v>
@@ -1742,7 +1820,7 @@
         <v>130</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>108</v>
@@ -1768,7 +1846,7 @@
         <v>131</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>109</v>
@@ -1791,10 +1869,10 @@
         <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>110</v>
@@ -1817,10 +1895,10 @@
         <v>49</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>111</v>
@@ -1846,7 +1924,7 @@
         <v>132</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>112</v>
@@ -1869,10 +1947,10 @@
         <v>78</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>113</v>
@@ -1898,7 +1976,7 @@
         <v>133</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>115</v>
@@ -1921,10 +1999,10 @@
         <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>114</v>
@@ -1950,7 +2028,7 @@
         <v>134</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>117</v>
@@ -1973,10 +2051,10 @@
         <v>22</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>135</v>
+        <v>206</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>119</v>
@@ -1999,10 +2077,10 @@
         <v>64</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>136</v>
+        <v>207</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>116</v>
@@ -2026,10 +2104,10 @@
         <v>89</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F28" s="4">
         <v>5</v>
@@ -2049,13 +2127,13 @@
         <v>35</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G29" s="4">
         <v>14.98</v>
@@ -2072,10 +2150,10 @@
         <v>78</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>120</v>
@@ -2095,10 +2173,10 @@
         <v>22</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>121</v>
@@ -2118,13 +2196,13 @@
         <v>85</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G32" s="4">
         <v>8.86</v>
@@ -2141,13 +2219,13 @@
         <v>47</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G33" s="4">
         <v>20.16</v>
@@ -2164,10 +2242,10 @@
         <v>6</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>122</v>
@@ -2187,10 +2265,10 @@
         <v>79</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>123</v>
@@ -2210,10 +2288,10 @@
         <v>80</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>124</v>
@@ -2233,13 +2311,13 @@
         <v>12</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G37" s="4">
         <v>5.21</v>
@@ -2256,10 +2334,10 @@
         <v>28</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>125</v>
@@ -2279,13 +2357,13 @@
         <v>81</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G39" s="4">
         <v>4.53</v>
@@ -2302,10 +2380,10 @@
         <v>82</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>126</v>
@@ -2325,13 +2403,13 @@
         <v>83</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G41" s="4">
         <v>4.8099999999999996</v>
@@ -2348,13 +2426,13 @@
         <v>84</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G42" s="4">
         <v>4.91</v>
@@ -2365,7 +2443,237 @@
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D44" s="4"/>
+      <c r="A44" s="1">
+        <v>41</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="G44" s="4">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>42</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="G45" s="4">
+        <v>4.6500000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>43</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G46" s="4">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>44</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G47" s="4">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>45</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G48" s="4">
+        <v>5.48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>46</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G49" s="4">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>47</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="F50" t="s">
+        <v>242</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>48</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>49</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>50</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F53" t="s">
+        <v>247</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C54" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2380,223 +2688,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G27"/>
+  <dimension ref="C1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="6" width="34.25" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="2:7" ht="16" x14ac:dyDescent="0.35">
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+    <row r="1" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="9"/>
-      <c r="C3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B4" s="9"/>
-      <c r="C4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B5" s="9"/>
-      <c r="C5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B6" s="9"/>
-      <c r="C6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B7" s="9"/>
-      <c r="C7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B8" s="9"/>
-      <c r="C8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B9" s="9"/>
-      <c r="C9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="16" x14ac:dyDescent="0.35">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B11" s="9"/>
-      <c r="C11" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="2:7" ht="16" x14ac:dyDescent="0.35">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B13" s="9"/>
-      <c r="C13" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="2:7" ht="16" x14ac:dyDescent="0.35">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="2:7" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B15" s="9"/>
-      <c r="C15" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C27" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update core game filter question; update lit review section
</commit_message>
<xml_diff>
--- a/method/CoreGame - titles and filter questions.xlsx
+++ b/method/CoreGame - titles and filter questions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\GitHub\MAPSS-Thesis\method\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\GitHub\MACS30200proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32730" yWindow="0" windowWidth="30700" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="34990" yWindow="0" windowWidth="30700" windowHeight="16980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="262">
   <si>
     <t>Game</t>
   </si>
@@ -426,21 +426,6 @@
     <t>In Mario Party DS, players:</t>
   </si>
   <si>
-    <r>
-      <t>In Nintendogs, which of the following is not an option in the game?</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
     <t>Civilization V is set in the:</t>
   </si>
   <si>
@@ -822,9 +807,6 @@
     <t>In Splatoon, what is incorrect about shapeshifting?</t>
   </si>
   <si>
-    <t>You shoot ink to change environment's color, You become a squid, You swim within the ink, You can replenish your ink supply</t>
-  </si>
-  <si>
     <t>You shoot ink to change environment's color</t>
   </si>
   <si>
@@ -867,9 +849,6 @@
     <t>Dragon Knight</t>
   </si>
   <si>
-    <t>What description is incorrect about Luke Triton in Professor Layton and the Curious Village?</t>
-  </si>
-  <si>
     <t>He is Layton's second son; He aspires to be a gentleman like Layton; He can talk to animals; He has very good appetite</t>
   </si>
   <si>
@@ -907,13 +886,34 @@
   </si>
   <si>
     <t>Which of the following is not a hero Class in Hearthstone?</t>
+  </si>
+  <si>
+    <t>What is incorrect about Luke Triton in Professor Layton and the Curious Village?</t>
+  </si>
+  <si>
+    <r>
+      <t>Regarding Nintendogs, which of the following is not an option in the game?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>You spit ink from your mouth, You look like a squid, You swim in the ink, You can replenish your ink supply</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -968,13 +968,26 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAF0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1007,7 +1020,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1025,6 +1038,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1049,6 +1079,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFAF0F0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1385,10 +1420,10 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1439,10 +1474,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>95</v>
@@ -1469,7 +1504,7 @@
         <v>94</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>98</v>
@@ -1493,10 +1528,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>99</v>
@@ -1520,10 +1555,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>118</v>
@@ -1547,10 +1582,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>100</v>
@@ -1574,10 +1609,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>96</v>
@@ -1601,10 +1636,10 @@
         <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>101</v>
@@ -1628,10 +1663,10 @@
         <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>102</v>
@@ -1658,7 +1693,7 @@
         <v>127</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>103</v>
@@ -1682,10 +1717,10 @@
         <v>22</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>97</v>
@@ -1709,10 +1744,10 @@
         <v>32</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>104</v>
@@ -1736,10 +1771,10 @@
         <v>35</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>105</v>
@@ -1766,7 +1801,7 @@
         <v>128</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>106</v>
@@ -1790,10 +1825,10 @@
         <v>28</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>129</v>
+        <v>260</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>107</v>
@@ -1817,10 +1852,10 @@
         <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>108</v>
@@ -1843,10 +1878,10 @@
         <v>45</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>109</v>
@@ -1869,10 +1904,10 @@
         <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>110</v>
@@ -1895,10 +1930,10 @@
         <v>49</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>111</v>
@@ -1921,10 +1956,10 @@
         <v>35</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>112</v>
@@ -1947,10 +1982,10 @@
         <v>78</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>113</v>
@@ -1973,10 +2008,10 @@
         <v>55</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>115</v>
@@ -1999,10 +2034,10 @@
         <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>114</v>
@@ -2025,10 +2060,10 @@
         <v>60</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>117</v>
@@ -2051,10 +2086,10 @@
         <v>22</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>119</v>
@@ -2077,10 +2112,10 @@
         <v>64</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>116</v>
@@ -2104,10 +2139,10 @@
         <v>89</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F28" s="4">
         <v>5</v>
@@ -2127,13 +2162,13 @@
         <v>35</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="G29" s="4">
         <v>14.98</v>
@@ -2150,10 +2185,10 @@
         <v>78</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>120</v>
@@ -2173,10 +2208,10 @@
         <v>22</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>121</v>
@@ -2196,13 +2231,13 @@
         <v>85</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G32" s="4">
         <v>8.86</v>
@@ -2219,13 +2254,13 @@
         <v>47</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="G33" s="4">
         <v>20.16</v>
@@ -2242,10 +2277,10 @@
         <v>6</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>122</v>
@@ -2265,10 +2300,10 @@
         <v>79</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>123</v>
@@ -2288,10 +2323,10 @@
         <v>80</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>124</v>
@@ -2311,13 +2346,13 @@
         <v>12</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="G37" s="4">
         <v>5.21</v>
@@ -2334,10 +2369,10 @@
         <v>28</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>125</v>
@@ -2357,13 +2392,13 @@
         <v>81</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G39" s="4">
         <v>4.53</v>
@@ -2380,10 +2415,10 @@
         <v>82</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>126</v>
@@ -2403,13 +2438,13 @@
         <v>83</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G41" s="4">
         <v>4.8099999999999996</v>
@@ -2426,13 +2461,13 @@
         <v>84</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G42" s="4">
         <v>4.91</v>
@@ -2447,19 +2482,19 @@
         <v>41</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G44" s="4">
         <v>5.9</v>
@@ -2470,19 +2505,19 @@
         <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>215</v>
-      </c>
       <c r="D45" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="G45" s="4">
         <v>4.6500000000000004</v>
@@ -2493,19 +2528,19 @@
         <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>217</v>
-      </c>
       <c r="D46" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G46" s="4">
         <v>22.7</v>
@@ -2516,19 +2551,19 @@
         <v>44</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>219</v>
-      </c>
       <c r="D47" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G47" s="4">
         <v>4.21</v>
@@ -2539,19 +2574,19 @@
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G48" s="4">
         <v>5.48</v>
@@ -2562,19 +2597,19 @@
         <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>223</v>
-      </c>
       <c r="D49" s="4" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G49" s="4">
         <v>5.19</v>
@@ -2585,19 +2620,19 @@
         <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F50" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>90</v>
@@ -2608,19 +2643,19 @@
         <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D51" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>243</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>90</v>
@@ -2631,19 +2666,19 @@
         <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>90</v>
@@ -2654,19 +2689,19 @@
         <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>228</v>
-      </c>
       <c r="D53" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F53" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>90</v>
@@ -2688,138 +2723,220 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:C25"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" style="9"/>
+    <col min="2" max="5" width="33.25" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="8.6640625" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C1" s="1" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C2" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C3" s="1" t="s">
+      <c r="D7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C4" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C5" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C6" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C7" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C8" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C10" s="1" t="s">
+      <c r="C15" s="12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C12" s="1" t="s">
+      <c r="D15" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C18" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C19" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C20" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C21" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C22" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C24" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C25" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C18" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>